<commit_message>
(etl) Data & ETL fixes/updates
1. Convert formulas to values (copy/paste as values/save)
2. Remove 2017 data from the 2019 file. The supplied file
   contained data for 2017 and 2019 but we only need to import
   2019 data because we imported the 2017 data last time
3. Add code to the ETL process to add the `t3xxx` questions
   to the CSV/JSON data
4. Convert references to `t3xxx` questions in the grouping
   sheet to numeric references (e.g: t3pbs --> 143 etc)
</commit_message>
<xml_diff>
--- a/data/GroupingsOBSQuestions2019.xlsx
+++ b/data/GroupingsOBSQuestions2019.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="176">
   <si>
     <t xml:space="preserve">Groupings for the OBS Questions (based on the 2015 Questionnaire)</t>
   </si>
@@ -132,10 +132,7 @@
     <t xml:space="preserve">Groupings for the OBS Questions (based on the 2019 and 2017 Questionnaire)</t>
   </si>
   <si>
-    <t xml:space="preserve">1-102, t3pbs, t3ebp, t3eb, t3iyr, t3myr, t3yer, t3ar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Note: We would also like to show the following indicators:</t>
+    <t xml:space="preserve">1-102, 143-149</t>
   </si>
   <si>
     <t xml:space="preserve">125-142</t>
@@ -144,67 +141,40 @@
     <t xml:space="preserve">107-124</t>
   </si>
   <si>
-    <t xml:space="preserve">t3pbs</t>
-  </si>
-  <si>
     <t xml:space="preserve">Legislative oversight</t>
   </si>
   <si>
     <t xml:space="preserve">107-118</t>
   </si>
   <si>
-    <t xml:space="preserve">t3ebp</t>
-  </si>
-  <si>
     <t xml:space="preserve">Supreme Audit Institution oversight</t>
   </si>
   <si>
     <t xml:space="preserve">119-124</t>
   </si>
   <si>
-    <t xml:space="preserve">t3eb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t3iyr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t3myr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54-58, t3pbs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t3yer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-53, t3ebp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t3ar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">59-63, t3eb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68-75, t3iyr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">76-83, t3myr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84-96, t3yer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">97-102,t3ar</t>
+    <t xml:space="preserve">54-58, 143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-53, 144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59-63, 145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68-75, 146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76-83, 147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84-96, 148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">97-102, 149</t>
   </si>
   <si>
     <t xml:space="preserve">Countries grouped by Region </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Note: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 New Countries</t>
   </si>
   <si>
     <t xml:space="preserve">East Asia &amp; Pacific</t>
@@ -698,7 +668,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -727,18 +697,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -747,11 +705,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -836,7 +794,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B42" activeCellId="1" sqref="J4:K12 B42"/>
+      <selection pane="topLeft" activeCell="B42" activeCellId="1" sqref="C11:C18 B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1054,27 +1012,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4:K12"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1013" min="3" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1014" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
@@ -1089,87 +1048,53 @@
       <c r="C4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="K4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" s="8" t="n">
-        <v>2017</v>
-      </c>
-      <c r="K5" s="9" t="n">
-        <v>2019</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>3.1</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>41</v>
+      <c r="B7" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>3.2</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>44</v>
+      <c r="B8" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="K8" s="0" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
-      <c r="J9" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="K9" s="0" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="4" t="s">
@@ -1178,12 +1103,6 @@
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -1193,13 +1112,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1210,16 +1123,10 @@
         <v>12</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>3</v>
       </c>
@@ -1227,10 +1134,10 @@
         <v>14</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>4</v>
       </c>
@@ -1241,7 +1148,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>5</v>
       </c>
@@ -1249,10 +1156,10 @@
         <v>18</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>6</v>
       </c>
@@ -1260,10 +1167,10 @@
         <v>20</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>7</v>
       </c>
@@ -1271,10 +1178,10 @@
         <v>22</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>8</v>
       </c>
@@ -1282,15 +1189,15 @@
         <v>24</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>1</v>
       </c>
@@ -1301,7 +1208,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>2</v>
       </c>
@@ -1312,7 +1219,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>3</v>
       </c>
@@ -1323,7 +1230,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>4</v>
       </c>
@@ -1334,15 +1241,6 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1360,10 +1258,10 @@
     <tabColor rgb="FF70AD47"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="1" sqref="J4:K12 C27"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="C11:C18 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1378,645 +1276,463 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B4" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
+      <c r="C4" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="D4" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="E4" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="F4" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="G4" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="H4" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="13" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="B5" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="E5" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="F5" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="G5" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="H5" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G5" s="7" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="F6" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="G6" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="H6" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="G6" s="7" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="E7" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="F7" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="G7" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="H7" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="G7" s="7" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="E8" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="F8" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="G8" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="H8" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="G8" s="7" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="E9" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="F9" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="G9" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="H9" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="7" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="E10" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="G10" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="H10" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="E10" s="7" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="D11" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="E11" s="5" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
+      <c r="G11" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="H11" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7" t="s">
+      <c r="D12" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="E12" s="5" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+      <c r="G12" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="H12" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7" t="s">
+      <c r="D13" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="E13" s="5" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
+      <c r="G13" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="H13" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7" t="s">
+      <c r="D14" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="G14" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7" t="s">
+      <c r="D15" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="G15" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="G16" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
+      <c r="D17" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="G17" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="12" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7" t="s">
+      <c r="B18" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
+      <c r="D18" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="G18" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7" t="s">
+      <c r="D19" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
+      <c r="G19" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="B18" s="7" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D20" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7" t="s">
+      <c r="G20" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
+      <c r="G21" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="B19" s="7" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G22" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G23" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7" t="s">
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G25" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G26" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7" t="s">
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G27" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7" t="s">
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G28" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7" t="s">
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G29" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7" t="s">
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G30" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7" t="s">
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G31" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7" t="s">
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G32" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="H23" s="7"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7" t="s">
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G33" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7" t="s">
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G34" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7" t="s">
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G35" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="H26" s="7"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G36" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="H27" s="7"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7" t="s">
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G37" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7" t="s">
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G38" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="H29" s="7"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7" t="s">
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G39" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="H30" s="7"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="H31" s="7"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="H32" s="7"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="H33" s="7"/>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="H34" s="7"/>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="H35" s="7"/>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="H36" s="7"/>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="H37" s="7"/>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="H38" s="7"/>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="H39" s="7"/>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="H40" s="7"/>
-    </row>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
(etl) North Macedonia --> Macedonia
Client wants to style this as Macedonia
</commit_message>
<xml_diff>
--- a/data/GroupingsOBSQuestions2019.xlsx
+++ b/data/GroupingsOBSQuestions2019.xlsx
@@ -794,7 +794,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B42" activeCellId="1" sqref="C11:C18 B42"/>
+      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1015,7 +1015,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11:C18"/>
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1261,7 +1261,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="C11:C18 A2"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
(etl) change group label, rebuild data
</commit_message>
<xml_diff>
--- a/data/GroupingsOBSQuestions2019.xlsx
+++ b/data/GroupingsOBSQuestions2019.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="177">
   <si>
     <t xml:space="preserve">Groupings for the OBS Questions (based on the 2015 Questionnaire)</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t xml:space="preserve">125-142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Role and Effectiveness of Oversight Institutions</t>
   </si>
   <si>
     <t xml:space="preserve">107-124</t>
@@ -1015,7 +1018,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1065,10 +1068,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1076,10 +1079,10 @@
         <v>3.1</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1087,10 +1090,10 @@
         <v>3.2</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1112,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1123,7 +1126,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1134,7 +1137,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1156,7 +1159,7 @@
         <v>18</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1167,7 +1170,7 @@
         <v>20</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1178,7 +1181,7 @@
         <v>22</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1189,7 +1192,7 @@
         <v>24</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1277,7 +1280,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="8"/>
@@ -1285,451 +1288,451 @@
     <row r="2" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G22" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G23" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G24" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G25" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G26" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G27" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G28" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G29" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G30" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G31" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G32" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G33" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G34" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G35" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G36" s="10" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G37" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G38" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G39" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>